<commit_message>
finished going through code for ms v08
</commit_message>
<xml_diff>
--- a/data/ideophones_coded_guessed_rated_simplified.xlsx
+++ b/data/ideophones_coded_guessed_rated_simplified.xlsx
@@ -461,7 +461,7 @@
         </is>
       </c>
       <c r="G2">
-        <v>0.8275862068965521</v>
+        <v>0.827586206896552</v>
       </c>
       <c r="H2">
         <v>3.28</v>
@@ -818,7 +818,7 @@
         <v>0</v>
       </c>
       <c r="N8">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9">
@@ -853,7 +853,7 @@
         </is>
       </c>
       <c r="G9">
-        <v>0.8275862068965521</v>
+        <v>0.827586206896552</v>
       </c>
       <c r="H9">
         <v>2.794444444444444</v>
@@ -1098,7 +1098,7 @@
         <v>0</v>
       </c>
       <c r="N13">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14">
@@ -1770,7 +1770,7 @@
         <v>0</v>
       </c>
       <c r="N25">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26">
@@ -2162,7 +2162,7 @@
         <v>0</v>
       </c>
       <c r="N32">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33">
@@ -2330,7 +2330,7 @@
         <v>0</v>
       </c>
       <c r="N35">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36">
@@ -2554,7 +2554,7 @@
         <v>0</v>
       </c>
       <c r="N39">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="40">
@@ -2778,7 +2778,7 @@
         <v>0</v>
       </c>
       <c r="N43">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="44">
@@ -3317,7 +3317,7 @@
         </is>
       </c>
       <c r="G53">
-        <v>0.8275862068965521</v>
+        <v>0.827586206896552</v>
       </c>
       <c r="H53">
         <v>2.542105263157895</v>
@@ -3429,7 +3429,7 @@
         </is>
       </c>
       <c r="G55">
-        <v>0.8275862068965521</v>
+        <v>0.827586206896552</v>
       </c>
       <c r="H55">
         <v>2.472222222222222</v>
@@ -5242,7 +5242,7 @@
         <v>0</v>
       </c>
       <c r="N87">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="88">
@@ -5466,7 +5466,7 @@
         <v>0</v>
       </c>
       <c r="N91">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="92">
@@ -5578,7 +5578,7 @@
         <v>0</v>
       </c>
       <c r="N93">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="94">
@@ -5802,7 +5802,7 @@
         <v>0</v>
       </c>
       <c r="N97">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="98">
@@ -6026,7 +6026,7 @@
         <v>0</v>
       </c>
       <c r="N101">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="102">
@@ -6362,7 +6362,7 @@
         <v>0</v>
       </c>
       <c r="N107">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="108">
@@ -6621,7 +6621,7 @@
         </is>
       </c>
       <c r="G112">
-        <v>0.8965517241379311</v>
+        <v>0.896551724137931</v>
       </c>
       <c r="H112">
         <v>3.244444444444445</v>
@@ -6642,7 +6642,7 @@
         <v>0</v>
       </c>
       <c r="N112">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="113">
@@ -8994,7 +8994,7 @@
         <v>0</v>
       </c>
       <c r="N154">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="155">
@@ -10674,7 +10674,7 @@
         <v>0</v>
       </c>
       <c r="N184">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="185">
@@ -11514,7 +11514,7 @@
         <v>0</v>
       </c>
       <c r="N199">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="200">
@@ -11794,7 +11794,7 @@
         <v>0</v>
       </c>
       <c r="N204">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="205">
@@ -12024,7 +12024,7 @@
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t xml:space="preserve">nààà</t>
+          <t>nààà</t>
         </is>
       </c>
       <c r="B209" t="inlineStr">
@@ -12634,7 +12634,7 @@
         <v>0</v>
       </c>
       <c r="N219">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="220">
@@ -12746,7 +12746,7 @@
         <v>0</v>
       </c>
       <c r="N221">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="222">
@@ -12920,7 +12920,7 @@
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t xml:space="preserve">kpìnàkpìnà</t>
+          <t>kpìnàkpìnà</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
@@ -13026,7 +13026,7 @@
         <v>0</v>
       </c>
       <c r="N226">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="227">

</xml_diff>